<commit_message>
Colorado Agg data update.
Colorado Agg data update.  Code standardization, water source type change.
</commit_message>
<xml_diff>
--- a/Colorado/AggregatedAmounts/CO_Aggregated Schema Mapping to WaDE_QA.xlsx
+++ b/Colorado/AggregatedAmounts/CO_Aggregated Schema Mapping to WaDE_QA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Colorado\AggregatedAmounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550E5AD4-B03F-4873-81CF-64CCD1B48DDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBADD76-3204-4037-B7A6-4186A8C7E7EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="645" activeTab="3" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="645" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="253">
   <si>
     <t>Name</t>
   </si>
@@ -680,9 +680,6 @@
     <t>State:</t>
   </si>
   <si>
-    <t>Organizaitons:</t>
-  </si>
-  <si>
     <t>Data Links:</t>
   </si>
   <si>
@@ -778,9 +775,6 @@
     <t>New VariableSpecific terms to add to db: ReservoirStorage, ForecastedRunoff, PrevMoStreamflow</t>
   </si>
   <si>
-    <t>New WaterSourceType terms to add to db: Lake, Creek, River, Spring</t>
-  </si>
-  <si>
     <t>CO_Supply</t>
   </si>
   <si>
@@ -792,6 +786,21 @@
   <si>
     <t>https://dwr.colorado.gov/about-us/contact-us/denver-office</t>
   </si>
+  <si>
+    <t>Duplicate Component ID, makes it hard to use as WaterSourceNativeID.</t>
+  </si>
+  <si>
+    <t>Water Source type is 'Surface Water'.</t>
+  </si>
+  <si>
+    <t>Organizations:</t>
+  </si>
+  <si>
+    <t>CSV format for Component ID is autoformatting and removing the leading '0' from the entries.</t>
+  </si>
+  <si>
+    <t>Only going to use Component ID as water source identifier for now, temporary fix.  Water source names in these instances seem familiar enough.</t>
+  </si>
 </sst>
 </file>
 
@@ -800,7 +809,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,14 +907,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1456,9 +1457,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1486,7 +1484,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1498,6 +1496,7 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1813,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE91C3C-F676-4E77-8227-802554E4B42D}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1837,82 +1836,103 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="97" t="s">
-        <v>213</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="97" t="s">
-        <v>214</v>
-      </c>
-      <c r="B6" s="104" t="s">
-        <v>219</v>
+        <v>213</v>
+      </c>
+      <c r="B6" s="103" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="101"/>
-      <c r="C7" s="100"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="99"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C8" s="100"/>
+      <c r="C8" s="99"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="99"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="100"/>
-      <c r="C10" s="100"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="99"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="100"/>
-      <c r="C11" s="100"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="99"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="97" t="s">
-        <v>215</v>
-      </c>
-      <c r="B13" s="100" t="s">
-        <v>217</v>
-      </c>
-      <c r="C13" s="100"/>
+        <v>214</v>
+      </c>
+      <c r="B13" s="99" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" s="99"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>220</v>
+      <c r="B14" s="99" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>244</v>
+      <c r="B15" s="99" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="100" t="s">
-        <v>245</v>
-      </c>
+      <c r="B16" s="99" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="99" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="113" t="s">
+        <v>252</v>
+      </c>
+      <c r="C19" s="98"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="98"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="98"/>
-      <c r="C20" s="99"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="98"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="98"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="97"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
+      <c r="B21" s="99"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="99"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="99"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2028,7 +2048,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="82" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
@@ -2188,7 +2208,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F9" s="84" t="s">
         <v>11</v>
@@ -2218,7 +2238,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F10" s="84" t="s">
         <v>11</v>
@@ -2250,7 +2270,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="95" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F11" s="84" t="s">
         <v>11</v>
@@ -2414,7 +2434,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F4" s="46"/>
       <c r="G4" s="34"/>
@@ -2470,7 +2490,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="94"/>
@@ -2498,7 +2518,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="94"/>
@@ -2582,7 +2602,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="96" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="94"/>
@@ -2610,7 +2630,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F11" s="26"/>
       <c r="G11" s="94"/>
@@ -2638,7 +2658,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="94"/>
@@ -2666,7 +2686,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="94"/>
@@ -2693,8 +2713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203F7812-755D-4EFC-B094-8BF895453DC0}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2825,7 +2845,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="95" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F5" s="84"/>
       <c r="G5" s="35"/>
@@ -2993,7 +3013,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="95" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F11" s="84"/>
       <c r="G11" s="35"/>
@@ -3093,7 +3113,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3196,7 +3216,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
@@ -3330,7 +3350,7 @@
         <v>11</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H8" s="92" t="s">
         <v>11</v>
@@ -3362,7 +3382,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H9" s="92" t="s">
         <v>11</v>
@@ -3430,7 +3450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E3782C-18A9-45D3-B018-D5B7F7291E9F}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -3534,7 +3554,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
@@ -3561,7 +3581,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="18"/>
-      <c r="E5" s="105" t="s">
+      <c r="E5" s="104" t="s">
         <v>102</v>
       </c>
       <c r="F5" s="21" t="s">
@@ -3594,7 +3614,7 @@
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>11</v>
@@ -3630,7 +3650,7 @@
         <v>11</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H7" s="92" t="s">
         <v>11</v>
@@ -3660,7 +3680,7 @@
         <v>11</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H8" s="92" t="s">
         <v>11</v>
@@ -3718,7 +3738,7 @@
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>11</v>
@@ -3898,8 +3918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E07544-54C6-4298-B1F4-AA27E9BE2694}">
   <dimension ref="A1:K16431"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4125,11 +4145,11 @@
       <c r="D9" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="103" t="s">
-        <v>222</v>
-      </c>
-      <c r="F9" s="107"/>
-      <c r="G9" s="108"/>
+      <c r="E9" s="102" t="s">
+        <v>221</v>
+      </c>
+      <c r="F9" s="106"/>
+      <c r="G9" s="107"/>
       <c r="H9" s="16" t="s">
         <v>11</v>
       </c>
@@ -4154,10 +4174,10 @@
       <c r="D10" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="102" t="s">
+      <c r="E10" s="101" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="109"/>
+      <c r="F10" s="108"/>
       <c r="G10" s="22"/>
       <c r="H10" s="16" t="s">
         <v>11</v>
@@ -4184,10 +4204,10 @@
         <v>11</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="F11" s="110"/>
-      <c r="G11" s="108"/>
+        <v>237</v>
+      </c>
+      <c r="F11" s="109"/>
+      <c r="G11" s="107"/>
       <c r="H11" s="16" t="s">
         <v>11</v>
       </c>
@@ -4212,10 +4232,10 @@
         <v>11</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="F12" s="110"/>
-      <c r="G12" s="108"/>
+        <v>224</v>
+      </c>
+      <c r="F12" s="109"/>
+      <c r="G12" s="107"/>
       <c r="H12" s="16" t="s">
         <v>11</v>
       </c>
@@ -4241,10 +4261,10 @@
         <v>11</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="F13" s="111"/>
-      <c r="G13" s="112"/>
+        <v>236</v>
+      </c>
+      <c r="F13" s="110"/>
+      <c r="G13" s="111"/>
       <c r="H13" s="16" t="s">
         <v>11</v>
       </c>
@@ -4304,8 +4324,8 @@
       <c r="F15" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="106" t="s">
-        <v>236</v>
+      <c r="G15" s="105" t="s">
+        <v>235</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>11</v>
@@ -4331,7 +4351,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="84" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F16" s="84" t="s">
         <v>11</v>
@@ -4456,7 +4476,7 @@
       <c r="D20" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="113">
+      <c r="E20" s="112">
         <v>44110</v>
       </c>
       <c r="F20" s="84"/>
@@ -4739,7 +4759,7 @@
         <v>15</v>
       </c>
       <c r="E29" s="84" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F29" s="84" t="s">
         <v>11</v>
@@ -4777,7 +4797,7 @@
         <v>11</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H30" s="16" t="s">
         <v>11</v>
@@ -4835,7 +4855,7 @@
         <v>15</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F32" s="84"/>
       <c r="G32" s="35"/>
@@ -4863,7 +4883,7 @@
         <v>15</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F33" s="84"/>
       <c r="G33" s="35"/>

</xml_diff>